<commit_message>
Chỉnh sửa kết quả của ZDT2 MOPSO trong bài
</commit_message>
<xml_diff>
--- a/Report/Table_MObj.xlsx
+++ b/Report/Table_MObj.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Le Xuan Thang\04. H5N1\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8395E9C-B615-4B15-B05E-99090988216A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA2F5B6-A7E6-4A44-BD95-BAE3AEB522E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="1" xr2:uid="{96C9E5A8-C2DF-4520-9AC5-ED16199CE618}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{96C9E5A8-C2DF-4520-9AC5-ED16199CE618}"/>
   </bookViews>
   <sheets>
     <sheet name="CEC2009" sheetId="2" r:id="rId1"/>
@@ -383,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -670,6 +670,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -986,17 +987,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4247A11F-D043-4316-97EF-7C3DD980BB96}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.75" style="2"/>
-    <col min="2" max="10" width="10.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.75" style="2" customWidth="1"/>
-    <col min="12" max="13" width="10.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.75" style="2"/>
+    <col min="1" max="1" width="8.69921875" style="2"/>
+    <col min="2" max="10" width="10.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.69921875" style="2" customWidth="1"/>
+    <col min="12" max="13" width="10.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.69921875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -1010,7 +1011,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="5" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1057,7 @@
       </c>
       <c r="AA4" s="11"/>
     </row>
-    <row r="5" spans="1:27" s="5" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>32</v>
@@ -1532,7 +1533,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="5" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1556,7 @@
       <c r="L11" s="48"/>
       <c r="M11" s="49"/>
     </row>
-    <row r="12" spans="1:27" s="5" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="24" t="s">
         <v>32</v>
@@ -1758,7 +1759,7 @@
         <v>0.74009999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:26" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>11</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>0.55230000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:26" s="5" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>0</v>
       </c>
@@ -1824,7 +1825,7 @@
       <c r="L18" s="54"/>
       <c r="M18" s="49"/>
     </row>
-    <row r="19" spans="1:26" s="5" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" s="5" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="13" t="s">
         <v>32</v>
@@ -2561,7 +2562,7 @@
       <c r="Y34" s="35"/>
       <c r="Z34" s="35"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
         <v>45</v>
       </c>
@@ -3068,7 +3069,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
         <v>45</v>
       </c>
@@ -3503,7 +3504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A53" s="61" t="s">
         <v>45</v>
       </c>
@@ -3566,40 +3567,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A6735E-E037-43E3-9DE8-91FCF6714F2A}">
   <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView showGridLines="0" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27:S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" style="2" customWidth="1"/>
     <col min="2" max="12" width="9" style="2"/>
     <col min="13" max="13" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="5.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="5.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.59765625" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="73" t="s">
         <v>20</v>
       </c>
@@ -3618,7 +3619,7 @@
       <c r="J4" s="66"/>
       <c r="K4" s="95"/>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" s="5" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="68"/>
       <c r="B5" s="69" t="s">
         <v>23</v>
@@ -3651,7 +3652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
         <v>32</v>
       </c>
@@ -3686,7 +3687,7 @@
         <v>7.3351925994275605E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
         <v>5</v>
       </c>
@@ -3721,7 +3722,7 @@
         <v>0.19963981877277301</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="75" t="s">
         <v>25</v>
       </c>
@@ -3756,7 +3757,7 @@
         <v>0.25885224224398101</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="73" t="s">
         <v>20</v>
       </c>
@@ -3775,7 +3776,7 @@
       <c r="J9" s="64"/>
       <c r="K9" s="94"/>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" s="5" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="68"/>
       <c r="B10" s="71" t="s">
         <v>23</v>
@@ -3808,7 +3809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
         <v>32</v>
       </c>
@@ -3843,24 +3844,24 @@
         <v>5.6422004470350798E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="27">
-        <v>2.16556072265295E-2</v>
+        <v>2.8311354182397701E-2</v>
       </c>
       <c r="C12" s="27">
-        <v>2.1628373934000499E-3</v>
+        <v>5.7500243860339299E-3</v>
       </c>
       <c r="D12" s="27">
-        <v>2.08306192087237E-2</v>
+        <v>2.4245472947044999E-2</v>
       </c>
       <c r="E12" s="27">
-        <v>1.9031562432145301E-2</v>
+        <v>2.4245472947044999E-2</v>
       </c>
       <c r="F12" s="27">
-        <v>2.5746773438782702E-2</v>
+        <v>3.2377235417750297E-2</v>
       </c>
       <c r="G12" s="27">
         <v>5.3528360075648103E-2</v>
@@ -3878,7 +3879,7 @@
         <v>0.21516518324772099</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="75" t="s">
         <v>25</v>
       </c>
@@ -3913,7 +3914,7 @@
         <v>0.17601367249268701</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="68" t="s">
         <v>20</v>
       </c>
@@ -3930,7 +3931,7 @@
       <c r="J14" s="77"/>
       <c r="K14" s="78"/>
     </row>
-    <row r="15" spans="1:11" s="5" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" s="5" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="68"/>
       <c r="B15" s="71" t="s">
         <v>23</v>
@@ -3952,8 +3953,14 @@
       <c r="I15" s="71"/>
       <c r="J15" s="71"/>
       <c r="K15" s="72"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
         <v>32</v>
       </c>
@@ -3977,6 +3984,12 @@
       <c r="I16" s="79"/>
       <c r="J16" s="79"/>
       <c r="K16" s="80"/>
+      <c r="M16" s="100"/>
+      <c r="N16" s="100"/>
+      <c r="O16" s="100"/>
+      <c r="P16" s="100"/>
+      <c r="Q16" s="100"/>
+      <c r="R16" s="100"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
@@ -4051,7 +4064,7 @@
       <c r="Y20" s="98"/>
       <c r="Z20" s="99"/>
     </row>
-    <row r="21" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="28.8" x14ac:dyDescent="0.25">
       <c r="L21" s="68"/>
       <c r="M21" s="69" t="s">
         <v>23</v>
@@ -4101,23 +4114,23 @@
         <v>32</v>
       </c>
       <c r="M22" s="85">
-        <f>RANK(B6,B$6:B$8,1)</f>
+        <f t="shared" ref="M22:Q24" si="0">RANK(B6,B$6:B$8,1)</f>
         <v>1</v>
       </c>
       <c r="N22" s="85">
-        <f>RANK(C6,C$6:C$8,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O22" s="85">
-        <f>RANK(D6,D$6:D$8,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P22" s="85">
-        <f>RANK(E6,E$6:E$8,1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="Q22" s="85">
-        <f>RANK(F6,F$6:F$8,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R22" s="41">
@@ -4129,23 +4142,23 @@
         <v>1</v>
       </c>
       <c r="T22" s="85">
-        <f>RANK(G6,G$6:G$8,1)</f>
+        <f t="shared" ref="T22:X24" si="1">RANK(G6,G$6:G$8,1)</f>
         <v>1</v>
       </c>
       <c r="U22" s="85">
-        <f>RANK(H6,H$6:H$8,1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="V22" s="85">
-        <f>RANK(I6,I$6:I$8,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="W22" s="85">
-        <f>RANK(J6,J$6:J$8,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="X22" s="85">
-        <f>RANK(K6,K$6:K$8,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Y22" s="41">
@@ -4162,59 +4175,59 @@
         <v>5</v>
       </c>
       <c r="M23" s="85">
-        <f>RANK(B7,B$6:B$8,1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N23" s="85">
-        <f>RANK(C7,C$6:C$8,1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="O23" s="85">
-        <f>RANK(D7,D$6:D$8,1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="P23" s="85">
-        <f>RANK(E7,E$6:E$8,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q23" s="85">
-        <f>RANK(F7,F$6:F$8,1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R23" s="41">
-        <f t="shared" ref="R23:R24" si="0">AVERAGE(M23:Q23)</f>
+        <f t="shared" ref="R23:R24" si="2">AVERAGE(M23:Q23)</f>
         <v>1.8</v>
       </c>
       <c r="S23" s="85">
-        <f t="shared" ref="S23:S24" si="1">RANK(R23,$R$22:$R$24,1)</f>
+        <f t="shared" ref="S23:S24" si="3">RANK(R23,$R$22:$R$24,1)</f>
         <v>2</v>
       </c>
       <c r="T23" s="85">
-        <f>RANK(G7,G$6:G$8,1)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="U23" s="85">
-        <f>RANK(H7,H$6:H$8,1)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V23" s="85">
-        <f>RANK(I7,I$6:I$8,1)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="W23" s="85">
-        <f>RANK(J7,J$6:J$8,1)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="X23" s="85">
-        <f>RANK(K7,K$6:K$8,1)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Y23" s="41">
-        <f t="shared" ref="Y23:Y24" si="2">AVERAGE(T23:X23)</f>
+        <f t="shared" ref="Y23:Y24" si="4">AVERAGE(T23:X23)</f>
         <v>2</v>
       </c>
       <c r="Z23" s="86">
-        <f t="shared" ref="Z23:Z24" si="3">RANK(Y23,$Y$22:$Y$24,1)</f>
+        <f t="shared" ref="Z23:Z24" si="5">RANK(Y23,$Y$22:$Y$24,1)</f>
         <v>2</v>
       </c>
     </row>
@@ -4223,59 +4236,59 @@
         <v>25</v>
       </c>
       <c r="M24" s="87">
-        <f>RANK(B8,B$6:B$8,1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="N24" s="87">
-        <f>RANK(C8,C$6:C$8,1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="O24" s="87">
-        <f>RANK(D8,D$6:D$8,1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="P24" s="87">
-        <f>RANK(E8,E$6:E$8,1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="Q24" s="87">
-        <f>RANK(F8,F$6:F$8,1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R24" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="S24" s="87">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="T24" s="87">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="T24" s="87">
-        <f>RANK(G8,G$6:G$8,1)</f>
-        <v>3</v>
-      </c>
       <c r="U24" s="87">
-        <f>RANK(H8,H$6:H$8,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V24" s="87">
-        <f>RANK(I8,I$6:I$8,1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="W24" s="87">
-        <f>RANK(J8,J$6:J$8,1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="X24" s="87">
-        <f>RANK(K8,K$6:K$8,1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="Y24" s="88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.6</v>
       </c>
       <c r="Z24" s="89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -4302,7 +4315,7 @@
       <c r="Y25" s="98"/>
       <c r="Z25" s="99"/>
     </row>
-    <row r="26" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="28.8" x14ac:dyDescent="0.25">
       <c r="L26" s="68"/>
       <c r="M26" s="71" t="s">
         <v>23</v>
@@ -4352,51 +4365,51 @@
         <v>32</v>
       </c>
       <c r="M27" s="85">
-        <f>RANK(B11,B$11:B$13,1)</f>
-        <v>2</v>
+        <f t="shared" ref="M27:Q29" si="6">RANK(B11,B$11:B$13,1)</f>
+        <v>1</v>
       </c>
       <c r="N27" s="85">
-        <f>RANK(C11,C$11:C$13,1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O27" s="85">
-        <f>RANK(D11,D$11:D$13,1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="P27" s="85">
-        <f>RANK(E11,E$11:E$13,1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="Q27" s="85">
-        <f>RANK(F11,F$11:F$13,1)</f>
-        <v>2</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="R27" s="41">
         <f>AVERAGE(M27:Q27)</f>
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
       <c r="S27" s="85">
         <f>RANK(R27,$R$27:$R$29,1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T27" s="85">
-        <f>RANK(G11,G$11:G$13,1)</f>
+        <f t="shared" ref="T27:X29" si="7">RANK(G11,G$11:G$13,1)</f>
         <v>1</v>
       </c>
       <c r="U27" s="85">
-        <f>RANK(H11,H$11:H$13,1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V27" s="85">
-        <f>RANK(I11,I$11:I$13,1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="W27" s="85">
-        <f>RANK(J11,J$11:J$13,1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="X27" s="85">
-        <f>RANK(K11,K$11:K$13,1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Y27" s="41">
@@ -4413,59 +4426,59 @@
         <v>5</v>
       </c>
       <c r="M28" s="85">
-        <f>RANK(B12,B$11:B$13,1)</f>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>2</v>
       </c>
       <c r="N28" s="85">
-        <f>RANK(C12,C$11:C$13,1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="O28" s="85">
-        <f>RANK(D12,D$11:D$13,1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P28" s="85">
-        <f>RANK(E12,E$11:E$13,1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q28" s="85">
-        <f>RANK(F12,F$11:F$13,1)</f>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>2</v>
       </c>
       <c r="R28" s="41">
-        <f t="shared" ref="R28:R29" si="4">AVERAGE(M28:Q28)</f>
-        <v>1.2</v>
+        <f t="shared" ref="R28:R29" si="8">AVERAGE(M28:Q28)</f>
+        <v>1.6</v>
       </c>
       <c r="S28" s="85">
-        <f t="shared" ref="S28:S29" si="5">RANK(R28,$R$27:$R$29,1)</f>
-        <v>1</v>
+        <f t="shared" ref="S28:S29" si="9">RANK(R28,$R$27:$R$29,1)</f>
+        <v>2</v>
       </c>
       <c r="T28" s="85">
-        <f>RANK(G12,G$11:G$13,1)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="U28" s="85">
-        <f>RANK(H12,H$11:H$13,1)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="V28" s="85">
-        <f>RANK(I12,I$11:I$13,1)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="W28" s="85">
-        <f>RANK(J12,J$11:J$13,1)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="X28" s="85">
-        <f>RANK(K12,K$11:K$13,1)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="Y28" s="41">
-        <f t="shared" ref="Y28:Y29" si="6">AVERAGE(T28:X28)</f>
+        <f t="shared" ref="Y28:Y29" si="10">AVERAGE(T28:X28)</f>
         <v>2.4</v>
       </c>
       <c r="Z28" s="86">
-        <f t="shared" ref="Z28:Z29" si="7">RANK(Y28,$Y$27:$Y$29,1)</f>
+        <f t="shared" ref="Z28:Z29" si="11">RANK(Y28,$Y$27:$Y$29,1)</f>
         <v>2</v>
       </c>
     </row>
@@ -4474,59 +4487,59 @@
         <v>25</v>
       </c>
       <c r="M29" s="87">
-        <f>RANK(B13,B$11:B$13,1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="N29" s="87">
-        <f>RANK(C13,C$11:C$13,1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="O29" s="87">
-        <f>RANK(D13,D$11:D$13,1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="P29" s="87">
-        <f>RANK(E13,E$11:E$13,1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="Q29" s="87">
-        <f>RANK(F13,F$11:F$13,1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="R29" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="S29" s="87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="T29" s="87">
-        <f>RANK(G13,G$11:G$13,1)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="U29" s="87">
-        <f>RANK(H13,H$11:H$13,1)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="V29" s="87">
-        <f>RANK(I13,I$11:I$13,1)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="W29" s="87">
-        <f>RANK(J13,J$11:J$13,1)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="X29" s="87">
-        <f>RANK(K13,K$11:K$13,1)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="Y29" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.6</v>
       </c>
       <c r="Z29" s="89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
     </row>
@@ -4551,7 +4564,7 @@
       <c r="Y30" s="83"/>
       <c r="Z30" s="84"/>
     </row>
-    <row r="31" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="28.8" x14ac:dyDescent="0.25">
       <c r="L31" s="68"/>
       <c r="M31" s="71" t="s">
         <v>23</v>
@@ -4587,23 +4600,23 @@
         <v>32</v>
       </c>
       <c r="M32" s="85">
-        <f>RANK(B16,B$16:B$18,1)</f>
+        <f t="shared" ref="M32:Q34" si="12">RANK(B16,B$16:B$18,1)</f>
         <v>1</v>
       </c>
       <c r="N32" s="85">
-        <f>RANK(C16,C$16:C$18,1)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="O32" s="85">
-        <f>RANK(D16,D$16:D$18,1)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="P32" s="85">
-        <f>RANK(E16,E$16:E$18,1)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="Q32" s="85">
-        <f>RANK(F16,F$16:F$18,1)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="R32" s="41">
@@ -4627,31 +4640,31 @@
         <v>5</v>
       </c>
       <c r="M33" s="85">
-        <f>RANK(B17,B$16:B$18,1)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="N33" s="85">
-        <f>RANK(C17,C$16:C$18,1)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="O33" s="85">
-        <f>RANK(D17,D$16:D$18,1)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="P33" s="85">
-        <f>RANK(E17,E$16:E$18,1)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="Q33" s="85">
-        <f>RANK(F17,F$16:F$18,1)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="R33" s="41">
-        <f t="shared" ref="R33:R34" si="8">AVERAGE(M33:Q33)</f>
+        <f t="shared" ref="R33:R34" si="13">AVERAGE(M33:Q33)</f>
         <v>1.8</v>
       </c>
       <c r="S33" s="85">
-        <f t="shared" ref="S33:S34" si="9">RANK(R33,$R$32:$R$34,1)</f>
+        <f t="shared" ref="S33:S34" si="14">RANK(R33,$R$32:$R$34,1)</f>
         <v>2</v>
       </c>
       <c r="T33" s="79"/>
@@ -4667,31 +4680,31 @@
         <v>25</v>
       </c>
       <c r="M34" s="87">
-        <f>RANK(B18,B$16:B$18,1)</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="N34" s="87">
-        <f>RANK(C18,C$16:C$18,1)</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="O34" s="87">
-        <f>RANK(D18,D$16:D$18,1)</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="P34" s="87">
-        <f>RANK(E18,E$16:E$18,1)</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="Q34" s="87">
-        <f>RANK(F18,F$16:F$18,1)</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="R34" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="S34" s="87">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="T34" s="81"/>

</xml_diff>